<commit_message>
Added more recent disaster csv and more new carrier file with column indicating which tiers to use in the util calc
</commit_message>
<xml_diff>
--- a/inputData/inputData03_US/fakeCarrierDataFEMA.xlsx
+++ b/inputData/inputData03_US/fakeCarrierDataFEMA.xlsx
@@ -9,17 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25620" windowHeight="12195"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25620" windowHeight="12195" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="fakeCarrierDataFEMA_for metrics" sheetId="1" r:id="rId1"/>
+    <sheet name="v2" sheetId="1" r:id="rId1"/>
+    <sheet name="v4" sheetId="2" r:id="rId2"/>
+    <sheet name="v3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="54">
   <si>
     <t>Contract</t>
   </si>
@@ -187,6 +189,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000000000"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -664,8 +669,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -989,13 +995,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -1023,12 +1029,12 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>4</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <f>E2/1.61/14968</f>
         <v>1.6183593322068444E-4</v>
       </c>
@@ -1043,22 +1049,22 @@
       </c>
       <c r="L2">
         <f>SUM(B2:B8)</f>
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="M2">
         <f>B2*C2</f>
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="N2">
         <f>B2*E2</f>
-        <v>23.4</v>
+        <v>39</v>
       </c>
       <c r="P2" t="s">
         <v>52</v>
       </c>
       <c r="Q2">
         <f>SUM(M2:M8)/L2</f>
-        <v>11.761194029850746</v>
+        <v>9.25</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -1066,28 +1072,28 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C3">
         <v>8</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <f t="shared" ref="D3:D41" si="0">E3/1.61/14968</f>
-        <v>1.4108773665393005E-4</v>
+        <v>1.4523737596728093E-4</v>
       </c>
       <c r="E3">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="F3" t="s">
         <v>7</v>
       </c>
       <c r="M3">
         <f t="shared" ref="M3:M40" si="1">B3*C3</f>
-        <v>72</v>
+        <v>136</v>
       </c>
       <c r="N3">
         <f t="shared" ref="N3:N40" si="2">B3*E3</f>
-        <v>30.599999999999998</v>
+        <v>59.5</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -1095,35 +1101,35 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C4">
-        <v>10</v>
-      </c>
-      <c r="D4">
-        <f t="shared" si="0"/>
-        <v>1.4938701528063181E-4</v>
+        <v>9</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>1.5353665459398271E-4</v>
       </c>
       <c r="E4">
-        <v>3.6</v>
+        <v>3.7</v>
       </c>
       <c r="F4" t="s">
         <v>7</v>
       </c>
       <c r="M4">
         <f t="shared" si="1"/>
-        <v>120</v>
+        <v>144</v>
       </c>
       <c r="N4">
         <f t="shared" si="2"/>
-        <v>43.2</v>
+        <v>59.2</v>
       </c>
       <c r="P4" t="s">
         <v>53</v>
       </c>
       <c r="Q4">
         <f>SUM(N2:N8)/L2</f>
-        <v>3.3746268656716421</v>
+        <v>3.5766666666666662</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -1131,12 +1137,12 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C5">
         <v>11</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <f t="shared" si="0"/>
         <v>1.4108773665393005E-4</v>
       </c>
@@ -1148,11 +1154,11 @@
       </c>
       <c r="M5">
         <f t="shared" si="1"/>
-        <v>88</v>
+        <v>33</v>
       </c>
       <c r="N5">
         <f t="shared" si="2"/>
-        <v>27.2</v>
+        <v>10.199999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -1160,12 +1166,12 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6">
         <v>13</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <f t="shared" si="0"/>
         <v>1.4523737596728093E-4</v>
       </c>
@@ -1177,11 +1183,11 @@
       </c>
       <c r="M6">
         <f t="shared" si="1"/>
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="N6">
         <f t="shared" si="2"/>
-        <v>31.5</v>
+        <v>24.5</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -1189,28 +1195,28 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C7">
         <v>15</v>
       </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
-        <v>1.2863881871387738E-4</v>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>1.2448917940052651E-4</v>
       </c>
       <c r="E7">
-        <v>3.1</v>
+        <v>3</v>
       </c>
       <c r="F7" t="s">
         <v>7</v>
       </c>
       <c r="M7">
         <f t="shared" si="1"/>
-        <v>180</v>
+        <v>60</v>
       </c>
       <c r="N7">
         <f t="shared" si="2"/>
-        <v>37.200000000000003</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -1218,28 +1224,28 @@
         <v>13</v>
       </c>
       <c r="B8">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C8">
         <v>17</v>
       </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>1.2448917940052651E-4</v>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4108773665393005E-4</v>
       </c>
       <c r="E8">
-        <v>3</v>
+        <v>3.4</v>
       </c>
       <c r="F8" t="s">
         <v>7</v>
       </c>
       <c r="M8">
         <f t="shared" si="1"/>
-        <v>187</v>
+        <v>51</v>
       </c>
       <c r="N8">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>10.199999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -1250,9 +1256,9 @@
         <v>100000</v>
       </c>
       <c r="C9">
-        <v>18</v>
-      </c>
-      <c r="D9">
+        <v>26</v>
+      </c>
+      <c r="D9" s="1">
         <f t="shared" si="0"/>
         <v>3.8176681682828125E-4</v>
       </c>
@@ -1273,12 +1279,12 @@
       <c r="C10">
         <v>4</v>
       </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
-        <v>1.1204026146047385E-4</v>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>1.3278845802722826E-4</v>
       </c>
       <c r="E10">
-        <v>2.7</v>
+        <v>3.2</v>
       </c>
       <c r="F10" t="s">
         <v>16</v>
@@ -1288,7 +1294,7 @@
       </c>
       <c r="L10">
         <f>SUM(B10:B16)</f>
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="M10">
         <f t="shared" si="1"/>
@@ -1296,14 +1302,14 @@
       </c>
       <c r="N10">
         <f t="shared" si="2"/>
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="P10" t="s">
         <v>52</v>
       </c>
       <c r="Q10">
         <f>SUM(M10:M16)/L10</f>
-        <v>11.149425287356323</v>
+        <v>13.012499999999999</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -1314,25 +1320,25 @@
         <v>15</v>
       </c>
       <c r="C11">
-        <v>7</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
-        <v>1.0789062214712296E-4</v>
+        <v>9</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1204026146047385E-4</v>
       </c>
       <c r="E11">
-        <v>2.6</v>
+        <v>2.7</v>
       </c>
       <c r="F11" t="s">
         <v>16</v>
       </c>
       <c r="M11">
         <f t="shared" si="1"/>
-        <v>105</v>
+        <v>135</v>
       </c>
       <c r="N11">
         <f t="shared" si="2"/>
-        <v>39</v>
+        <v>40.5</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -1340,28 +1346,28 @@
         <v>18</v>
       </c>
       <c r="B12">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C12">
-        <v>8</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>9.9591343520421204E-5</v>
+        <v>10</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>1.2448917940052651E-4</v>
       </c>
       <c r="E12">
-        <v>2.4</v>
+        <v>3</v>
       </c>
       <c r="F12" t="s">
         <v>16</v>
       </c>
       <c r="M12">
         <f t="shared" si="1"/>
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="N12">
         <f t="shared" si="2"/>
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -1369,35 +1375,35 @@
         <v>19</v>
       </c>
       <c r="B13">
+        <v>14</v>
+      </c>
+      <c r="C13">
         <v>15</v>
       </c>
-      <c r="C13">
-        <v>9</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="0"/>
-        <v>9.5441704207070312E-5</v>
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1204026146047385E-4</v>
       </c>
       <c r="E13">
-        <v>2.2999999999999998</v>
+        <v>2.7</v>
       </c>
       <c r="F13" t="s">
         <v>16</v>
       </c>
       <c r="M13">
         <f t="shared" si="1"/>
-        <v>135</v>
+        <v>210</v>
       </c>
       <c r="N13">
         <f t="shared" si="2"/>
-        <v>34.5</v>
+        <v>37.800000000000004</v>
       </c>
       <c r="P13" t="s">
         <v>53</v>
       </c>
       <c r="Q13">
         <f>SUM(N10:N16)/L10</f>
-        <v>2.4218390804597703</v>
+        <v>2.7875000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -1410,12 +1416,12 @@
       <c r="C14">
         <v>20</v>
       </c>
-      <c r="D14">
-        <f t="shared" si="0"/>
-        <v>9.9591343520421204E-5</v>
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0789062214712296E-4</v>
       </c>
       <c r="E14">
-        <v>2.4</v>
+        <v>2.6</v>
       </c>
       <c r="F14" t="s">
         <v>16</v>
@@ -1426,7 +1432,7 @@
       </c>
       <c r="N14">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -1434,28 +1440,28 @@
         <v>21</v>
       </c>
       <c r="B15">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C15">
         <v>22</v>
       </c>
-      <c r="D15">
-        <f t="shared" si="0"/>
-        <v>9.1292064893719446E-5</v>
+      <c r="D15" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0374098283377208E-4</v>
       </c>
       <c r="E15">
-        <v>2.2000000000000002</v>
+        <v>2.5</v>
       </c>
       <c r="F15" t="s">
         <v>16</v>
       </c>
       <c r="M15">
         <f t="shared" si="1"/>
-        <v>198</v>
+        <v>154</v>
       </c>
       <c r="N15">
         <f t="shared" si="2"/>
-        <v>19.8</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -1468,12 +1474,12 @@
       <c r="C16">
         <v>24</v>
       </c>
-      <c r="D16">
-        <f t="shared" si="0"/>
-        <v>9.5441704207070312E-5</v>
+      <c r="D16" s="1">
+        <f t="shared" si="0"/>
+        <v>9.9591343520421204E-5</v>
       </c>
       <c r="E16">
-        <v>2.2999999999999998</v>
+        <v>2.4</v>
       </c>
       <c r="F16" t="s">
         <v>16</v>
@@ -1484,7 +1490,7 @@
       </c>
       <c r="N16">
         <f t="shared" si="2"/>
-        <v>18.399999999999999</v>
+        <v>19.2</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -1495,9 +1501,9 @@
         <v>100000</v>
       </c>
       <c r="C17">
-        <v>25</v>
-      </c>
-      <c r="D17">
+        <v>26</v>
+      </c>
+      <c r="D17" s="1">
         <f t="shared" si="0"/>
         <v>2.8632511262121095E-4</v>
       </c>
@@ -1513,12 +1519,12 @@
         <v>24</v>
       </c>
       <c r="B18">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C18">
         <v>4</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="1">
         <f t="shared" si="0"/>
         <v>1.4938701528063181E-4</v>
       </c>
@@ -1533,22 +1539,22 @@
       </c>
       <c r="L18">
         <f>SUM(B18:B24)</f>
-        <v>98</v>
+        <v>60</v>
       </c>
       <c r="M18">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="N18">
         <f t="shared" si="2"/>
-        <v>43.2</v>
+        <v>28.8</v>
       </c>
       <c r="P18" t="s">
         <v>52</v>
       </c>
       <c r="Q18">
         <f>SUM(M18:M24)/L18</f>
-        <v>14.897959183673469</v>
+        <v>12.033333333333333</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -1556,12 +1562,12 @@
         <v>26</v>
       </c>
       <c r="B19">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C19">
-        <v>6</v>
-      </c>
-      <c r="D19">
+        <v>9</v>
+      </c>
+      <c r="D19" s="1">
         <f t="shared" si="0"/>
         <v>1.5768629390733354E-4</v>
       </c>
@@ -1573,11 +1579,11 @@
       </c>
       <c r="M19">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>108</v>
       </c>
       <c r="N19">
         <f t="shared" si="2"/>
-        <v>26.599999999999998</v>
+        <v>45.599999999999994</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
@@ -1585,12 +1591,12 @@
         <v>27</v>
       </c>
       <c r="B20">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C20">
-        <v>9</v>
-      </c>
-      <c r="D20">
+        <v>11</v>
+      </c>
+      <c r="D20" s="1">
         <f t="shared" si="0"/>
         <v>1.4523737596728093E-4</v>
       </c>
@@ -1602,11 +1608,11 @@
       </c>
       <c r="M20">
         <f t="shared" si="1"/>
-        <v>27</v>
+        <v>110</v>
       </c>
       <c r="N20">
         <f t="shared" si="2"/>
-        <v>10.5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
@@ -1614,12 +1620,12 @@
         <v>28</v>
       </c>
       <c r="B21">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C21">
-        <v>12</v>
-      </c>
-      <c r="D21">
+        <v>14</v>
+      </c>
+      <c r="D21" s="1">
         <f t="shared" si="0"/>
         <v>1.4938701528063181E-4</v>
       </c>
@@ -1631,18 +1637,18 @@
       </c>
       <c r="M21">
         <f t="shared" si="1"/>
-        <v>180</v>
+        <v>140</v>
       </c>
       <c r="N21">
         <f t="shared" si="2"/>
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="P21" t="s">
         <v>53</v>
       </c>
       <c r="Q21">
         <f>SUM(N18:N24)/L18</f>
-        <v>3.4336734693877551</v>
+        <v>3.5433333333333326</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
@@ -1650,12 +1656,12 @@
         <v>29</v>
       </c>
       <c r="B22">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C22">
         <v>15</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="1">
         <f t="shared" si="0"/>
         <v>1.4108773665393005E-4</v>
       </c>
@@ -1667,11 +1673,11 @@
       </c>
       <c r="M22">
         <f t="shared" si="1"/>
-        <v>255</v>
+        <v>120</v>
       </c>
       <c r="N22">
         <f t="shared" si="2"/>
-        <v>57.8</v>
+        <v>27.2</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -1679,12 +1685,12 @@
         <v>30</v>
       </c>
       <c r="B23">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C23">
-        <v>19</v>
-      </c>
-      <c r="D23">
+        <v>16</v>
+      </c>
+      <c r="D23" s="1">
         <f t="shared" si="0"/>
         <v>1.4523737596728093E-4</v>
       </c>
@@ -1696,11 +1702,11 @@
       </c>
       <c r="M23">
         <f t="shared" si="1"/>
-        <v>380</v>
+        <v>112</v>
       </c>
       <c r="N23">
         <f t="shared" si="2"/>
-        <v>70</v>
+        <v>24.5</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
@@ -1708,12 +1714,12 @@
         <v>31</v>
       </c>
       <c r="B24">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="C24">
-        <v>22</v>
-      </c>
-      <c r="D24">
+        <v>20</v>
+      </c>
+      <c r="D24" s="1">
         <f t="shared" si="0"/>
         <v>1.2863881871387738E-4</v>
       </c>
@@ -1725,11 +1731,11 @@
       </c>
       <c r="M24">
         <f t="shared" si="1"/>
-        <v>528</v>
+        <v>100</v>
       </c>
       <c r="N24">
         <f t="shared" si="2"/>
-        <v>74.400000000000006</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
@@ -1740,9 +1746,9 @@
         <v>100000</v>
       </c>
       <c r="C25">
-        <v>23</v>
-      </c>
-      <c r="D25">
+        <v>26</v>
+      </c>
+      <c r="D25" s="1">
         <f t="shared" si="0"/>
         <v>3.7761717751493034E-4</v>
       </c>
@@ -1763,12 +1769,12 @@
       <c r="C26">
         <v>4</v>
       </c>
-      <c r="D26">
-        <f t="shared" si="0"/>
-        <v>1.6183593322068444E-4</v>
+      <c r="D26" s="1">
+        <f t="shared" si="0"/>
+        <v>1.3278845802722826E-4</v>
       </c>
       <c r="E26">
-        <v>3.9</v>
+        <v>3.2</v>
       </c>
       <c r="F26" t="s">
         <v>34</v>
@@ -1778,7 +1784,7 @@
       </c>
       <c r="L26">
         <f>SUM(B26:B32)</f>
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="M26">
         <f t="shared" si="1"/>
@@ -1786,14 +1792,14 @@
       </c>
       <c r="N26">
         <f t="shared" si="2"/>
-        <v>50.699999999999996</v>
+        <v>41.6</v>
       </c>
       <c r="P26" t="s">
         <v>52</v>
       </c>
       <c r="Q26">
         <f>SUM(M26:M32)/L26</f>
-        <v>8.7297297297297298</v>
+        <v>13.875</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
@@ -1804,25 +1810,25 @@
         <v>16</v>
       </c>
       <c r="C27">
-        <v>5</v>
-      </c>
-      <c r="D27">
-        <f t="shared" si="0"/>
-        <v>1.4108773665393005E-4</v>
+        <v>10</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" si="0"/>
+        <v>1.2448917940052651E-4</v>
       </c>
       <c r="E27">
-        <v>3.4</v>
+        <v>3</v>
       </c>
       <c r="F27" t="s">
         <v>34</v>
       </c>
       <c r="M27">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>160</v>
       </c>
       <c r="N27">
         <f t="shared" si="2"/>
-        <v>54.4</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
@@ -1833,25 +1839,25 @@
         <v>19</v>
       </c>
       <c r="C28">
-        <v>7</v>
-      </c>
-      <c r="D28">
-        <f t="shared" si="0"/>
-        <v>1.3278845802722826E-4</v>
+        <v>15</v>
+      </c>
+      <c r="D28" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0789062214712296E-4</v>
       </c>
       <c r="E28">
-        <v>3.2</v>
+        <v>2.6</v>
       </c>
       <c r="F28" t="s">
         <v>34</v>
       </c>
       <c r="M28">
         <f t="shared" si="1"/>
-        <v>133</v>
+        <v>285</v>
       </c>
       <c r="N28">
         <f t="shared" si="2"/>
-        <v>60.800000000000004</v>
+        <v>49.4</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
@@ -1862,32 +1868,32 @@
         <v>5</v>
       </c>
       <c r="C29">
-        <v>9</v>
-      </c>
-      <c r="D29">
-        <f t="shared" si="0"/>
-        <v>1.4523737596728093E-4</v>
+        <v>16</v>
+      </c>
+      <c r="D29" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1204026146047385E-4</v>
       </c>
       <c r="E29">
-        <v>3.5</v>
+        <v>2.7</v>
       </c>
       <c r="F29" t="s">
         <v>34</v>
       </c>
       <c r="M29">
         <f t="shared" si="1"/>
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="N29">
         <f t="shared" si="2"/>
-        <v>17.5</v>
+        <v>13.5</v>
       </c>
       <c r="P29" t="s">
         <v>53</v>
       </c>
       <c r="Q29">
         <f>SUM(N26:N32)/L26</f>
-        <v>3.3972972972972979</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
@@ -1898,25 +1904,25 @@
         <v>16</v>
       </c>
       <c r="C30">
-        <v>15</v>
-      </c>
-      <c r="D30">
-        <f t="shared" si="0"/>
-        <v>1.3278845802722826E-4</v>
+        <v>18</v>
+      </c>
+      <c r="D30" s="1">
+        <f t="shared" si="0"/>
+        <v>9.1292064893719446E-5</v>
       </c>
       <c r="E30">
-        <v>3.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F30" t="s">
         <v>34</v>
       </c>
       <c r="M30">
         <f t="shared" si="1"/>
-        <v>240</v>
+        <v>288</v>
       </c>
       <c r="N30">
         <f t="shared" si="2"/>
-        <v>51.2</v>
+        <v>35.200000000000003</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
@@ -1924,28 +1930,28 @@
         <v>39</v>
       </c>
       <c r="B31">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C31">
-        <v>18</v>
-      </c>
-      <c r="D31">
-        <f t="shared" si="0"/>
-        <v>1.6183593322068444E-4</v>
+        <v>19</v>
+      </c>
+      <c r="D31" s="1">
+        <f t="shared" si="0"/>
+        <v>1.2033954008717561E-4</v>
       </c>
       <c r="E31">
-        <v>3.9</v>
+        <v>2.9</v>
       </c>
       <c r="F31" t="s">
         <v>34</v>
       </c>
       <c r="M31">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>95</v>
       </c>
       <c r="N31">
         <f t="shared" si="2"/>
-        <v>7.8</v>
+        <v>14.5</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
@@ -1953,28 +1959,28 @@
         <v>40</v>
       </c>
       <c r="B32">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C32">
-        <v>20</v>
-      </c>
-      <c r="D32">
-        <f t="shared" si="0"/>
-        <v>1.2448917940052651E-4</v>
+        <v>25</v>
+      </c>
+      <c r="D32" s="1">
+        <f t="shared" si="0"/>
+        <v>9.5441704207070312E-5</v>
       </c>
       <c r="E32">
-        <v>3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F32" t="s">
         <v>34</v>
       </c>
       <c r="M32">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>150</v>
       </c>
       <c r="N32">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>13.799999999999999</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
@@ -1985,9 +1991,9 @@
         <v>100000</v>
       </c>
       <c r="C33">
-        <v>21</v>
-      </c>
-      <c r="D33">
+        <v>26</v>
+      </c>
+      <c r="D33" s="1">
         <f t="shared" si="0"/>
         <v>3.2782150575471979E-4</v>
       </c>
@@ -2003,17 +2009,17 @@
         <v>42</v>
       </c>
       <c r="B34">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C34">
         <v>4</v>
       </c>
-      <c r="D34">
-        <f t="shared" si="0"/>
-        <v>1.2863881871387738E-4</v>
+      <c r="D34" s="1">
+        <f t="shared" si="0"/>
+        <v>1.5768629390733354E-4</v>
       </c>
       <c r="E34">
-        <v>3.1</v>
+        <v>3.8</v>
       </c>
       <c r="F34" t="s">
         <v>43</v>
@@ -2023,22 +2029,22 @@
       </c>
       <c r="L34">
         <f>SUM(B34:B40)</f>
-        <v>69</v>
+        <v>100</v>
       </c>
       <c r="M34">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="N34">
         <f t="shared" si="2"/>
-        <v>18.600000000000001</v>
+        <v>57</v>
       </c>
       <c r="P34" t="s">
         <v>52</v>
       </c>
       <c r="Q34">
         <f>SUM(M34:M40)/L34</f>
-        <v>11.231884057971014</v>
+        <v>11.9</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
@@ -2049,25 +2055,25 @@
         <v>16</v>
       </c>
       <c r="C35">
-        <v>7</v>
-      </c>
-      <c r="D35">
-        <f t="shared" si="0"/>
-        <v>1.3278845802722826E-4</v>
+        <v>8</v>
+      </c>
+      <c r="D35" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4938701528063181E-4</v>
       </c>
       <c r="E35">
-        <v>3.2</v>
+        <v>3.6</v>
       </c>
       <c r="F35" t="s">
         <v>43</v>
       </c>
       <c r="M35">
         <f t="shared" si="1"/>
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="N35">
         <f t="shared" si="2"/>
-        <v>51.2</v>
+        <v>57.6</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
@@ -2075,28 +2081,28 @@
         <v>45</v>
       </c>
       <c r="B36">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C36">
-        <v>9</v>
-      </c>
-      <c r="D36">
-        <f t="shared" si="0"/>
-        <v>1.2863881871387738E-4</v>
+        <v>10</v>
+      </c>
+      <c r="D36" s="1">
+        <f t="shared" si="0"/>
+        <v>1.5353665459398271E-4</v>
       </c>
       <c r="E36">
-        <v>3.1</v>
+        <v>3.7</v>
       </c>
       <c r="F36" t="s">
         <v>43</v>
       </c>
       <c r="M36">
         <f t="shared" si="1"/>
-        <v>45</v>
+        <v>120</v>
       </c>
       <c r="N36">
         <f t="shared" si="2"/>
-        <v>15.5</v>
+        <v>44.400000000000006</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
@@ -2104,35 +2110,35 @@
         <v>46</v>
       </c>
       <c r="B37">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C37">
-        <v>10</v>
-      </c>
-      <c r="D37">
-        <f t="shared" si="0"/>
-        <v>1.3278845802722826E-4</v>
+        <v>13</v>
+      </c>
+      <c r="D37" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4938701528063181E-4</v>
       </c>
       <c r="E37">
-        <v>3.2</v>
+        <v>3.6</v>
       </c>
       <c r="F37" t="s">
         <v>43</v>
       </c>
       <c r="M37">
         <f t="shared" si="1"/>
-        <v>120</v>
+        <v>195</v>
       </c>
       <c r="N37">
         <f t="shared" si="2"/>
-        <v>38.400000000000006</v>
+        <v>54</v>
       </c>
       <c r="P37" t="s">
         <v>53</v>
       </c>
       <c r="Q37">
         <f>SUM(N34:N40)/L34</f>
-        <v>2.9971014492753625</v>
+        <v>3.5129999999999999</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
@@ -2140,28 +2146,28 @@
         <v>47</v>
       </c>
       <c r="B38">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C38">
         <v>14</v>
       </c>
-      <c r="D38">
-        <f t="shared" si="0"/>
-        <v>1.2033954008717561E-4</v>
+      <c r="D38" s="1">
+        <f t="shared" si="0"/>
+        <v>1.3278845802722826E-4</v>
       </c>
       <c r="E38">
-        <v>2.9</v>
+        <v>3.2</v>
       </c>
       <c r="F38" t="s">
         <v>43</v>
       </c>
       <c r="M38">
         <f t="shared" si="1"/>
-        <v>84</v>
+        <v>210</v>
       </c>
       <c r="N38">
         <f t="shared" si="2"/>
-        <v>17.399999999999999</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
@@ -2169,28 +2175,28 @@
         <v>48</v>
       </c>
       <c r="B39">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C39">
-        <v>15</v>
-      </c>
-      <c r="D39">
-        <f t="shared" si="0"/>
-        <v>1.1618990077382472E-4</v>
+        <v>16</v>
+      </c>
+      <c r="D39" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4108773665393005E-4</v>
       </c>
       <c r="E39">
-        <v>2.8</v>
+        <v>3.4</v>
       </c>
       <c r="F39" t="s">
         <v>43</v>
       </c>
       <c r="M39">
         <f t="shared" si="1"/>
-        <v>135</v>
+        <v>192</v>
       </c>
       <c r="N39">
         <f t="shared" si="2"/>
-        <v>25.2</v>
+        <v>40.799999999999997</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
@@ -2201,25 +2207,25 @@
         <v>15</v>
       </c>
       <c r="C40">
-        <v>17</v>
-      </c>
-      <c r="D40">
-        <f t="shared" si="0"/>
-        <v>1.1204026146047385E-4</v>
+        <v>19</v>
+      </c>
+      <c r="D40" s="1">
+        <f t="shared" si="0"/>
+        <v>1.3693809734057914E-4</v>
       </c>
       <c r="E40">
-        <v>2.7</v>
+        <v>3.3</v>
       </c>
       <c r="F40" t="s">
         <v>43</v>
       </c>
       <c r="M40">
         <f t="shared" si="1"/>
-        <v>255</v>
+        <v>285</v>
       </c>
       <c r="N40">
         <f t="shared" si="2"/>
-        <v>40.5</v>
+        <v>49.5</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
@@ -2230,9 +2236,2535 @@
         <v>100000</v>
       </c>
       <c r="C41">
+        <v>26</v>
+      </c>
+      <c r="D41" s="1">
+        <f t="shared" si="0"/>
+        <v>3.7761717751493034E-4</v>
+      </c>
+      <c r="E41">
+        <v>9.1</v>
+      </c>
+      <c r="F41" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="24.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1">
+        <f>E2/1.61/14968</f>
+        <v>1.6183593322068444E-4</v>
+      </c>
+      <c r="E2">
+        <v>3.9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" t="s">
+        <v>51</v>
+      </c>
+      <c r="L2">
+        <f>SUM(B2:B8)</f>
+        <v>60</v>
+      </c>
+      <c r="M2">
+        <f>B2*C2</f>
+        <v>40</v>
+      </c>
+      <c r="N2">
+        <f>B2*E2</f>
+        <v>39</v>
+      </c>
+      <c r="P2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q2">
+        <f>SUM(M2:M8)/L2</f>
+        <v>9.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>17</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" ref="D3:D41" si="0">E3/1.61/14968</f>
+        <v>1.4523737596728093E-4</v>
+      </c>
+      <c r="E3">
+        <v>3.5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M40" si="1">B3*C3</f>
+        <v>136</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N40" si="2">B3*E3</f>
+        <v>59.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>16</v>
+      </c>
+      <c r="C4">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>1.5353665459398271E-4</v>
+      </c>
+      <c r="E4">
+        <v>3.7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="1"/>
+        <v>144</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="2"/>
+        <v>59.2</v>
+      </c>
+      <c r="P4" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q4">
+        <f>SUM(N2:N8)/L2</f>
+        <v>3.5766666666666662</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4108773665393005E-4</v>
+      </c>
+      <c r="E5">
+        <v>3.4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="2"/>
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4523737596728093E-4</v>
+      </c>
+      <c r="E6">
+        <v>3.5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="1"/>
+        <v>91</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="2"/>
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>15</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>1.2448917940052651E-4</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>17</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4108773665393005E-4</v>
+      </c>
+      <c r="E8">
+        <v>3.4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>7</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="2"/>
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>100000</v>
+      </c>
+      <c r="C9">
+        <v>26</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>3.8176681682828125E-4</v>
+      </c>
+      <c r="E9">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>1.3278845802722826E-4</v>
+      </c>
+      <c r="E10">
+        <v>3.2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" t="s">
+        <v>51</v>
+      </c>
+      <c r="L10">
+        <f>SUM(B10:B16)</f>
+        <v>160</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="2"/>
+        <v>64</v>
+      </c>
+      <c r="P10" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q10">
+        <f>SUM(M10:M16)/L10</f>
+        <v>13.012499999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>30</v>
+      </c>
+      <c r="C11">
+        <v>9</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1204026146047385E-4</v>
+      </c>
+      <c r="E11">
+        <v>2.7</v>
+      </c>
+      <c r="F11" t="s">
+        <v>16</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="1"/>
+        <v>270</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="2"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>18</v>
       </c>
-      <c r="D41">
+      <c r="B12">
+        <v>42</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>1.2448917940052651E-4</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12" t="s">
+        <v>16</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="1"/>
+        <v>420</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="2"/>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13">
+        <v>28</v>
+      </c>
+      <c r="C13">
+        <v>15</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1204026146047385E-4</v>
+      </c>
+      <c r="E13">
+        <v>2.7</v>
+      </c>
+      <c r="F13" t="s">
+        <v>16</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="1"/>
+        <v>420</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="2"/>
+        <v>75.600000000000009</v>
+      </c>
+      <c r="P13" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q13">
+        <f>SUM(N10:N16)/L10</f>
+        <v>2.7875000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>20</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0789062214712296E-4</v>
+      </c>
+      <c r="E14">
+        <v>2.6</v>
+      </c>
+      <c r="F14" t="s">
+        <v>16</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="1"/>
+        <v>200</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>22</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0374098283377208E-4</v>
+      </c>
+      <c r="E15">
+        <v>2.5</v>
+      </c>
+      <c r="F15" t="s">
+        <v>16</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="1"/>
+        <v>308</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16">
+        <v>16</v>
+      </c>
+      <c r="C16">
+        <v>24</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="0"/>
+        <v>9.9591343520421204E-5</v>
+      </c>
+      <c r="E16">
+        <v>2.4</v>
+      </c>
+      <c r="F16" t="s">
+        <v>16</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="1"/>
+        <v>384</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="2"/>
+        <v>38.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17">
+        <v>100000</v>
+      </c>
+      <c r="C17">
+        <v>26</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="0"/>
+        <v>2.8632511262121095E-4</v>
+      </c>
+      <c r="E17">
+        <v>6.9</v>
+      </c>
+      <c r="F17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18">
+        <v>8</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4938701528063181E-4</v>
+      </c>
+      <c r="E18">
+        <v>3.6</v>
+      </c>
+      <c r="F18" t="s">
+        <v>25</v>
+      </c>
+      <c r="K18" t="s">
+        <v>51</v>
+      </c>
+      <c r="L18">
+        <f>SUM(B18:B24)</f>
+        <v>60</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="2"/>
+        <v>28.8</v>
+      </c>
+      <c r="P18" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q18">
+        <f>SUM(M18:M24)/L18</f>
+        <v>12.033333333333333</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19">
+        <v>12</v>
+      </c>
+      <c r="C19">
+        <v>9</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="0"/>
+        <v>1.5768629390733354E-4</v>
+      </c>
+      <c r="E19">
+        <v>3.8</v>
+      </c>
+      <c r="F19" t="s">
+        <v>25</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="1"/>
+        <v>108</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="2"/>
+        <v>45.599999999999994</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20">
+        <v>10</v>
+      </c>
+      <c r="C20">
+        <v>11</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4523737596728093E-4</v>
+      </c>
+      <c r="E20">
+        <v>3.5</v>
+      </c>
+      <c r="F20" t="s">
+        <v>25</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21">
+        <v>10</v>
+      </c>
+      <c r="C21">
+        <v>14</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4938701528063181E-4</v>
+      </c>
+      <c r="E21">
+        <v>3.6</v>
+      </c>
+      <c r="F21" t="s">
+        <v>25</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="1"/>
+        <v>140</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="P21" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q21">
+        <f>SUM(N18:N24)/L18</f>
+        <v>3.5433333333333326</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22">
+        <v>8</v>
+      </c>
+      <c r="C22">
+        <v>15</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4108773665393005E-4</v>
+      </c>
+      <c r="E22">
+        <v>3.4</v>
+      </c>
+      <c r="F22" t="s">
+        <v>25</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="2"/>
+        <v>27.2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23">
+        <v>7</v>
+      </c>
+      <c r="C23">
+        <v>16</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4523737596728093E-4</v>
+      </c>
+      <c r="E23">
+        <v>3.5</v>
+      </c>
+      <c r="F23" t="s">
+        <v>25</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="1"/>
+        <v>112</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="2"/>
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24">
+        <v>5</v>
+      </c>
+      <c r="C24">
+        <v>20</v>
+      </c>
+      <c r="D24" s="1">
+        <f t="shared" si="0"/>
+        <v>1.2863881871387738E-4</v>
+      </c>
+      <c r="E24">
+        <v>3.1</v>
+      </c>
+      <c r="F24" t="s">
+        <v>25</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="2"/>
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25">
+        <v>100000</v>
+      </c>
+      <c r="C25">
+        <v>26</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" si="0"/>
+        <v>3.7761717751493034E-4</v>
+      </c>
+      <c r="E25">
+        <v>9.1</v>
+      </c>
+      <c r="F25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26">
+        <v>26</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" si="0"/>
+        <v>1.3278845802722826E-4</v>
+      </c>
+      <c r="E26">
+        <v>3.2</v>
+      </c>
+      <c r="F26" t="s">
+        <v>34</v>
+      </c>
+      <c r="K26" t="s">
+        <v>51</v>
+      </c>
+      <c r="L26">
+        <f>SUM(B26:B32)</f>
+        <v>160</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="1"/>
+        <v>104</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="2"/>
+        <v>83.2</v>
+      </c>
+      <c r="P26" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q26">
+        <f>SUM(M26:M32)/L26</f>
+        <v>13.875</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27">
+        <v>32</v>
+      </c>
+      <c r="C27">
+        <v>10</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" si="0"/>
+        <v>1.2448917940052651E-4</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
+      </c>
+      <c r="F27" t="s">
+        <v>34</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="1"/>
+        <v>320</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="2"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28">
+        <v>38</v>
+      </c>
+      <c r="C28">
+        <v>15</v>
+      </c>
+      <c r="D28" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0789062214712296E-4</v>
+      </c>
+      <c r="E28">
+        <v>2.6</v>
+      </c>
+      <c r="F28" t="s">
+        <v>34</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="1"/>
+        <v>570</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="2"/>
+        <v>98.8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29">
+        <v>10</v>
+      </c>
+      <c r="C29">
+        <v>16</v>
+      </c>
+      <c r="D29" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1204026146047385E-4</v>
+      </c>
+      <c r="E29">
+        <v>2.7</v>
+      </c>
+      <c r="F29" t="s">
+        <v>34</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="P29" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q29">
+        <f>SUM(N26:N32)/L26</f>
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30">
+        <v>32</v>
+      </c>
+      <c r="C30">
+        <v>18</v>
+      </c>
+      <c r="D30" s="1">
+        <f t="shared" si="0"/>
+        <v>9.1292064893719446E-5</v>
+      </c>
+      <c r="E30">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F30" t="s">
+        <v>34</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="1"/>
+        <v>576</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="2"/>
+        <v>70.400000000000006</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31">
+        <v>10</v>
+      </c>
+      <c r="C31">
+        <v>19</v>
+      </c>
+      <c r="D31" s="1">
+        <f t="shared" si="0"/>
+        <v>1.2033954008717561E-4</v>
+      </c>
+      <c r="E31">
+        <v>2.9</v>
+      </c>
+      <c r="F31" t="s">
+        <v>34</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="1"/>
+        <v>190</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32">
+        <v>12</v>
+      </c>
+      <c r="C32">
+        <v>25</v>
+      </c>
+      <c r="D32" s="1">
+        <f t="shared" si="0"/>
+        <v>9.5441704207070312E-5</v>
+      </c>
+      <c r="E32">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F32" t="s">
+        <v>34</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="2"/>
+        <v>27.599999999999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33">
+        <v>100000</v>
+      </c>
+      <c r="C33">
+        <v>26</v>
+      </c>
+      <c r="D33" s="1">
+        <f t="shared" si="0"/>
+        <v>3.2782150575471979E-4</v>
+      </c>
+      <c r="E33">
+        <v>7.9</v>
+      </c>
+      <c r="F33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34">
+        <v>15</v>
+      </c>
+      <c r="C34">
+        <v>4</v>
+      </c>
+      <c r="D34" s="1">
+        <f t="shared" si="0"/>
+        <v>1.5768629390733354E-4</v>
+      </c>
+      <c r="E34">
+        <v>3.8</v>
+      </c>
+      <c r="F34" t="s">
+        <v>43</v>
+      </c>
+      <c r="K34" t="s">
+        <v>51</v>
+      </c>
+      <c r="L34">
+        <f>SUM(B34:B40)</f>
+        <v>100</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="2"/>
+        <v>57</v>
+      </c>
+      <c r="P34" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q34">
+        <f>SUM(M34:M40)/L34</f>
+        <v>11.9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35">
+        <v>16</v>
+      </c>
+      <c r="C35">
+        <v>8</v>
+      </c>
+      <c r="D35" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4938701528063181E-4</v>
+      </c>
+      <c r="E35">
+        <v>3.6</v>
+      </c>
+      <c r="F35" t="s">
+        <v>43</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="1"/>
+        <v>128</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="2"/>
+        <v>57.6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36">
+        <v>12</v>
+      </c>
+      <c r="C36">
+        <v>10</v>
+      </c>
+      <c r="D36" s="1">
+        <f t="shared" si="0"/>
+        <v>1.5353665459398271E-4</v>
+      </c>
+      <c r="E36">
+        <v>3.7</v>
+      </c>
+      <c r="F36" t="s">
+        <v>43</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="2"/>
+        <v>44.400000000000006</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37">
+        <v>15</v>
+      </c>
+      <c r="C37">
+        <v>13</v>
+      </c>
+      <c r="D37" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4938701528063181E-4</v>
+      </c>
+      <c r="E37">
+        <v>3.6</v>
+      </c>
+      <c r="F37" t="s">
+        <v>43</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="1"/>
+        <v>195</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="2"/>
+        <v>54</v>
+      </c>
+      <c r="P37" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q37">
+        <f>SUM(N34:N40)/L34</f>
+        <v>3.5129999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38">
+        <v>15</v>
+      </c>
+      <c r="C38">
+        <v>14</v>
+      </c>
+      <c r="D38" s="1">
+        <f t="shared" si="0"/>
+        <v>1.3278845802722826E-4</v>
+      </c>
+      <c r="E38">
+        <v>3.2</v>
+      </c>
+      <c r="F38" t="s">
+        <v>43</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="1"/>
+        <v>210</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39">
+        <v>12</v>
+      </c>
+      <c r="C39">
+        <v>16</v>
+      </c>
+      <c r="D39" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4108773665393005E-4</v>
+      </c>
+      <c r="E39">
+        <v>3.4</v>
+      </c>
+      <c r="F39" t="s">
+        <v>43</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="1"/>
+        <v>192</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="2"/>
+        <v>40.799999999999997</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40">
+        <v>15</v>
+      </c>
+      <c r="C40">
+        <v>19</v>
+      </c>
+      <c r="D40" s="1">
+        <f t="shared" si="0"/>
+        <v>1.3693809734057914E-4</v>
+      </c>
+      <c r="E40">
+        <v>3.3</v>
+      </c>
+      <c r="F40" t="s">
+        <v>43</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="1"/>
+        <v>285</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="2"/>
+        <v>49.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>50</v>
+      </c>
+      <c r="B41">
+        <v>100000</v>
+      </c>
+      <c r="C41">
+        <v>26</v>
+      </c>
+      <c r="D41" s="1">
+        <f t="shared" si="0"/>
+        <v>3.7761717751493034E-4</v>
+      </c>
+      <c r="E41">
+        <v>9.1</v>
+      </c>
+      <c r="F41" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="24.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>20</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1">
+        <f>E2/1.61/14968</f>
+        <v>1.6183593322068444E-4</v>
+      </c>
+      <c r="E2">
+        <v>3.9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" t="s">
+        <v>51</v>
+      </c>
+      <c r="L2">
+        <f>SUM(B2:B8)</f>
+        <v>120</v>
+      </c>
+      <c r="M2">
+        <f>B2*C2</f>
+        <v>80</v>
+      </c>
+      <c r="N2">
+        <f>B2*E2</f>
+        <v>78</v>
+      </c>
+      <c r="P2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q2">
+        <f>SUM(M2:M8)/L2</f>
+        <v>9.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>34</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" ref="D3:D41" si="0">E3/1.61/14968</f>
+        <v>1.4523737596728093E-4</v>
+      </c>
+      <c r="E3">
+        <v>3.5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M40" si="1">B3*C3</f>
+        <v>272</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N40" si="2">B3*E3</f>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>32</v>
+      </c>
+      <c r="C4">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>1.5353665459398271E-4</v>
+      </c>
+      <c r="E4">
+        <v>3.7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="1"/>
+        <v>288</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="2"/>
+        <v>118.4</v>
+      </c>
+      <c r="P4" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q4">
+        <f>SUM(N2:N8)/L2</f>
+        <v>3.5766666666666662</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4108773665393005E-4</v>
+      </c>
+      <c r="E5">
+        <v>3.4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="1"/>
+        <v>66</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="2"/>
+        <v>20.399999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4523737596728093E-4</v>
+      </c>
+      <c r="E6">
+        <v>3.5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="1"/>
+        <v>182</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>15</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>1.2448917940052651E-4</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>17</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4108773665393005E-4</v>
+      </c>
+      <c r="E8">
+        <v>3.4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>7</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="1"/>
+        <v>102</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="2"/>
+        <v>20.399999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>100000</v>
+      </c>
+      <c r="C9">
+        <v>26</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>3.8176681682828125E-4</v>
+      </c>
+      <c r="E9">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>1.3278845802722826E-4</v>
+      </c>
+      <c r="E10">
+        <v>3.2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" t="s">
+        <v>51</v>
+      </c>
+      <c r="L10">
+        <f>SUM(B10:B16)</f>
+        <v>160</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="2"/>
+        <v>64</v>
+      </c>
+      <c r="P10" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q10">
+        <f>SUM(M10:M16)/L10</f>
+        <v>13.012499999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>30</v>
+      </c>
+      <c r="C11">
+        <v>9</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1204026146047385E-4</v>
+      </c>
+      <c r="E11">
+        <v>2.7</v>
+      </c>
+      <c r="F11" t="s">
+        <v>16</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="1"/>
+        <v>270</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="2"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12">
+        <v>42</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>1.2448917940052651E-4</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12" t="s">
+        <v>16</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="1"/>
+        <v>420</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="2"/>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13">
+        <v>28</v>
+      </c>
+      <c r="C13">
+        <v>15</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1204026146047385E-4</v>
+      </c>
+      <c r="E13">
+        <v>2.7</v>
+      </c>
+      <c r="F13" t="s">
+        <v>16</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="1"/>
+        <v>420</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="2"/>
+        <v>75.600000000000009</v>
+      </c>
+      <c r="P13" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q13">
+        <f>SUM(N10:N16)/L10</f>
+        <v>2.7875000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>20</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0789062214712296E-4</v>
+      </c>
+      <c r="E14">
+        <v>2.6</v>
+      </c>
+      <c r="F14" t="s">
+        <v>16</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="1"/>
+        <v>200</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>22</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0374098283377208E-4</v>
+      </c>
+      <c r="E15">
+        <v>2.5</v>
+      </c>
+      <c r="F15" t="s">
+        <v>16</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="1"/>
+        <v>308</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16">
+        <v>16</v>
+      </c>
+      <c r="C16">
+        <v>24</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="0"/>
+        <v>9.9591343520421204E-5</v>
+      </c>
+      <c r="E16">
+        <v>2.4</v>
+      </c>
+      <c r="F16" t="s">
+        <v>16</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="1"/>
+        <v>384</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="2"/>
+        <v>38.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17">
+        <v>100000</v>
+      </c>
+      <c r="C17">
+        <v>26</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="0"/>
+        <v>2.8632511262121095E-4</v>
+      </c>
+      <c r="E17">
+        <v>6.9</v>
+      </c>
+      <c r="F17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4938701528063181E-4</v>
+      </c>
+      <c r="E18">
+        <v>3.6</v>
+      </c>
+      <c r="F18" t="s">
+        <v>25</v>
+      </c>
+      <c r="K18" t="s">
+        <v>51</v>
+      </c>
+      <c r="L18">
+        <f>SUM(B18:B24)</f>
+        <v>120</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="2"/>
+        <v>57.6</v>
+      </c>
+      <c r="P18" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q18">
+        <f>SUM(M18:M24)/L18</f>
+        <v>12.033333333333333</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19">
+        <v>24</v>
+      </c>
+      <c r="C19">
+        <v>9</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="0"/>
+        <v>1.5768629390733354E-4</v>
+      </c>
+      <c r="E19">
+        <v>3.8</v>
+      </c>
+      <c r="F19" t="s">
+        <v>25</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="1"/>
+        <v>216</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="2"/>
+        <v>91.199999999999989</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20">
+        <v>20</v>
+      </c>
+      <c r="C20">
+        <v>11</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4523737596728093E-4</v>
+      </c>
+      <c r="E20">
+        <v>3.5</v>
+      </c>
+      <c r="F20" t="s">
+        <v>25</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="1"/>
+        <v>220</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <v>14</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4938701528063181E-4</v>
+      </c>
+      <c r="E21">
+        <v>3.6</v>
+      </c>
+      <c r="F21" t="s">
+        <v>25</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="1"/>
+        <v>280</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="2"/>
+        <v>72</v>
+      </c>
+      <c r="P21" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q21">
+        <f>SUM(N18:N24)/L18</f>
+        <v>3.5433333333333326</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22">
+        <v>16</v>
+      </c>
+      <c r="C22">
+        <v>15</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4108773665393005E-4</v>
+      </c>
+      <c r="E22">
+        <v>3.4</v>
+      </c>
+      <c r="F22" t="s">
+        <v>25</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="1"/>
+        <v>240</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="2"/>
+        <v>54.4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23">
+        <v>14</v>
+      </c>
+      <c r="C23">
+        <v>16</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4523737596728093E-4</v>
+      </c>
+      <c r="E23">
+        <v>3.5</v>
+      </c>
+      <c r="F23" t="s">
+        <v>25</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="1"/>
+        <v>224</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24">
+        <v>10</v>
+      </c>
+      <c r="C24">
+        <v>20</v>
+      </c>
+      <c r="D24" s="1">
+        <f t="shared" si="0"/>
+        <v>1.2863881871387738E-4</v>
+      </c>
+      <c r="E24">
+        <v>3.1</v>
+      </c>
+      <c r="F24" t="s">
+        <v>25</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="1"/>
+        <v>200</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25">
+        <v>100000</v>
+      </c>
+      <c r="C25">
+        <v>26</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" si="0"/>
+        <v>3.7761717751493034E-4</v>
+      </c>
+      <c r="E25">
+        <v>9.1</v>
+      </c>
+      <c r="F25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26">
+        <v>26</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" si="0"/>
+        <v>1.3278845802722826E-4</v>
+      </c>
+      <c r="E26">
+        <v>3.2</v>
+      </c>
+      <c r="F26" t="s">
+        <v>34</v>
+      </c>
+      <c r="K26" t="s">
+        <v>51</v>
+      </c>
+      <c r="L26">
+        <f>SUM(B26:B32)</f>
+        <v>160</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="1"/>
+        <v>104</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="2"/>
+        <v>83.2</v>
+      </c>
+      <c r="P26" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q26">
+        <f>SUM(M26:M32)/L26</f>
+        <v>13.875</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27">
+        <v>32</v>
+      </c>
+      <c r="C27">
+        <v>10</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" si="0"/>
+        <v>1.2448917940052651E-4</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
+      </c>
+      <c r="F27" t="s">
+        <v>34</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="1"/>
+        <v>320</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="2"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28">
+        <v>38</v>
+      </c>
+      <c r="C28">
+        <v>15</v>
+      </c>
+      <c r="D28" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0789062214712296E-4</v>
+      </c>
+      <c r="E28">
+        <v>2.6</v>
+      </c>
+      <c r="F28" t="s">
+        <v>34</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="1"/>
+        <v>570</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="2"/>
+        <v>98.8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29">
+        <v>10</v>
+      </c>
+      <c r="C29">
+        <v>16</v>
+      </c>
+      <c r="D29" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1204026146047385E-4</v>
+      </c>
+      <c r="E29">
+        <v>2.7</v>
+      </c>
+      <c r="F29" t="s">
+        <v>34</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="P29" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q29">
+        <f>SUM(N26:N32)/L26</f>
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30">
+        <v>32</v>
+      </c>
+      <c r="C30">
+        <v>18</v>
+      </c>
+      <c r="D30" s="1">
+        <f t="shared" si="0"/>
+        <v>9.1292064893719446E-5</v>
+      </c>
+      <c r="E30">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F30" t="s">
+        <v>34</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="1"/>
+        <v>576</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="2"/>
+        <v>70.400000000000006</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31">
+        <v>10</v>
+      </c>
+      <c r="C31">
+        <v>19</v>
+      </c>
+      <c r="D31" s="1">
+        <f t="shared" si="0"/>
+        <v>1.2033954008717561E-4</v>
+      </c>
+      <c r="E31">
+        <v>2.9</v>
+      </c>
+      <c r="F31" t="s">
+        <v>34</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="1"/>
+        <v>190</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32">
+        <v>12</v>
+      </c>
+      <c r="C32">
+        <v>25</v>
+      </c>
+      <c r="D32" s="1">
+        <f t="shared" si="0"/>
+        <v>9.5441704207070312E-5</v>
+      </c>
+      <c r="E32">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F32" t="s">
+        <v>34</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="2"/>
+        <v>27.599999999999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33">
+        <v>100000</v>
+      </c>
+      <c r="C33">
+        <v>26</v>
+      </c>
+      <c r="D33" s="1">
+        <f t="shared" si="0"/>
+        <v>3.2782150575471979E-4</v>
+      </c>
+      <c r="E33">
+        <v>7.9</v>
+      </c>
+      <c r="F33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34">
+        <v>30</v>
+      </c>
+      <c r="C34">
+        <v>4</v>
+      </c>
+      <c r="D34" s="1">
+        <f t="shared" si="0"/>
+        <v>1.5768629390733354E-4</v>
+      </c>
+      <c r="E34">
+        <v>3.8</v>
+      </c>
+      <c r="F34" t="s">
+        <v>43</v>
+      </c>
+      <c r="K34" t="s">
+        <v>51</v>
+      </c>
+      <c r="L34">
+        <f>SUM(B34:B40)</f>
+        <v>200</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="2"/>
+        <v>114</v>
+      </c>
+      <c r="P34" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q34">
+        <f>SUM(M34:M40)/L34</f>
+        <v>11.9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35">
+        <v>32</v>
+      </c>
+      <c r="C35">
+        <v>8</v>
+      </c>
+      <c r="D35" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4938701528063181E-4</v>
+      </c>
+      <c r="E35">
+        <v>3.6</v>
+      </c>
+      <c r="F35" t="s">
+        <v>43</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="1"/>
+        <v>256</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="2"/>
+        <v>115.2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36">
+        <v>24</v>
+      </c>
+      <c r="C36">
+        <v>10</v>
+      </c>
+      <c r="D36" s="1">
+        <f t="shared" si="0"/>
+        <v>1.5353665459398271E-4</v>
+      </c>
+      <c r="E36">
+        <v>3.7</v>
+      </c>
+      <c r="F36" t="s">
+        <v>43</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="1"/>
+        <v>240</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="2"/>
+        <v>88.800000000000011</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37">
+        <v>30</v>
+      </c>
+      <c r="C37">
+        <v>13</v>
+      </c>
+      <c r="D37" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4938701528063181E-4</v>
+      </c>
+      <c r="E37">
+        <v>3.6</v>
+      </c>
+      <c r="F37" t="s">
+        <v>43</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="1"/>
+        <v>390</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="2"/>
+        <v>108</v>
+      </c>
+      <c r="P37" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q37">
+        <f>SUM(N34:N40)/L34</f>
+        <v>3.5129999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38">
+        <v>30</v>
+      </c>
+      <c r="C38">
+        <v>14</v>
+      </c>
+      <c r="D38" s="1">
+        <f t="shared" si="0"/>
+        <v>1.3278845802722826E-4</v>
+      </c>
+      <c r="E38">
+        <v>3.2</v>
+      </c>
+      <c r="F38" t="s">
+        <v>43</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="1"/>
+        <v>420</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="2"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39">
+        <v>24</v>
+      </c>
+      <c r="C39">
+        <v>16</v>
+      </c>
+      <c r="D39" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4108773665393005E-4</v>
+      </c>
+      <c r="E39">
+        <v>3.4</v>
+      </c>
+      <c r="F39" t="s">
+        <v>43</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="1"/>
+        <v>384</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="2"/>
+        <v>81.599999999999994</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40">
+        <v>30</v>
+      </c>
+      <c r="C40">
+        <v>19</v>
+      </c>
+      <c r="D40" s="1">
+        <f t="shared" si="0"/>
+        <v>1.3693809734057914E-4</v>
+      </c>
+      <c r="E40">
+        <v>3.3</v>
+      </c>
+      <c r="F40" t="s">
+        <v>43</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="1"/>
+        <v>570</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="2"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>50</v>
+      </c>
+      <c r="B41">
+        <v>100000</v>
+      </c>
+      <c r="C41">
+        <v>26</v>
+      </c>
+      <c r="D41" s="1">
         <f t="shared" si="0"/>
         <v>3.7761717751493034E-4</v>
       </c>

</xml_diff>